<commit_message>
Add recommendation systems and robot learning job categories, update metalearning curriculum
- Added 7 ML Engineer (Recommendation Systems) jobs from TikTok, Amazon, Meta, Netflix
- Added 10 ML Engineer (Robot Learning) jobs from various robotics companies
- Added skills_aggregate2.md sections for both new categories with skill frequencies
- Updated 1metalearning.md with:
  - Job postings analysis for recommendation systems (12 skills)
  - Recommendation systems concepts, facts, and procedures
  - Note explaining robot learning barrier to entry (PhD/3-6 yrs required)
  - University curricula research (Stanford CS229, CMU ML, MIT 6.036)
  - Online courses research (6 courses: Andrew Ng, FastAI, FSDL, MLOps Zoomcamp, Made With ML)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/career/job_listings.xlsx
+++ b/career/job_listings.xlsx
@@ -495,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3539,6 +3539,805 @@
       <c r="I69" t="inlineStr">
         <is>
           <t>Python, C++, ROS, data pipelines, computer vision, perception systems, embedded systems, distributed processing</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>TikTok</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer, TikTok Recommendation</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>San Jose, CA</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>ML Engineer (Recommendation Systems)</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>https://careers.tiktok.com/position/7112323775379343623/detail</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Master's or PhD in Computer Science, Machine Learning, or related field; experience with large-scale recommendation systems; strong publication record preferred</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Build large-scale (10M-100M) recommendation algorithms and systems; design user interest models for short and long-term preferences; develop CTR/CVR prediction models; build real-time data pipelines and feature engineering</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Python, C++, PyTorch/TensorFlow, distributed systems, deep learning, recommendation algorithms, real-time ML systems, feature engineering, A/B testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Lead AI/ML Engineer, Recommendation Systems (Prime Video)</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Seattle, WA</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>ML Engineer (Recommendation Systems)</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>https://amazon.jobs/en/jobs/3065041/lead-ai-ml-engineer-recommendation-systems</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>PhD or Master's degree in CS, ML, or related field; 6+ years applied research experience; 5+ years building ML models for business applications</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Develop AI solutions for personalization; design and conduct offline and online A/B experiments; stay current with latest modeling techniques; lead technical direction for recommendation systems</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Python, PyTorch/TensorFlow, deep learning, recommendation systems, A/B testing, causal inference, distributed computing, AWS, Spark</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer - Personalization</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Seattle, WA</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>ML Engineer (Recommendation Systems)</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>https://www.amazon.jobs/en/jobs/3065042/machine-learning-engineer-personalization</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Master's or PhD in CS, CE, ML or related field; 3+ years building ML models for business applications; experience with recommendation and search systems</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Develop ML models for recommendation and search systems using deep learning, online learning, and optimization; tackle cold-start problems with foundation models; build scalable personalization systems</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Python, PyTorch/TensorFlow, deep learning, online learning, optimization, recommendation systems, foundation models, AWS, distributed systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer, Amazon Music ML &amp; Personalization</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>San Francisco, CA</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>ML Engineer (Recommendation Systems)</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>https://www.amazon.jobs/en/jobs/3004439/machine-learning-engineer-amazon-music-ml-personalization</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>BS/MS in Computer Science, ML, or related field; experience with recommendation systems and personalization; familiarity with music/audio domain a plus</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Deliver personalized recommendations for millions of Amazon Music customers globally; own models underlying all recommendation surfaces across mobile, web, and Alexa; build data pipelines and approximate nearest neighbor services</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Python, PyTorch/TensorFlow, recommendation systems, approximate nearest neighbors, data pipelines, A/B testing, AWS, distributed systems, audio/music ML</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Meta</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Senior Machine Learning Engineer, Recommendation Systems</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>FAANG</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Menlo Park, CA</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>ML Engineer (Recommendation Systems)</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>https://www.metacareers.com/jobs/2472910023050061</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>BS/MS/PhD in Computer Science, ML, or related field; 5+ years experience with recommendation systems; experience at companies like Google, Meta, or Twitter preferred</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Architect, design, implement, and test large-scale distributed recommendation systems end-to-end; lead team building recommendation product for Short Videos in Facebook Newsfeed; own inventory design, content retrieval, ranking stages, delivery, and ML infra</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Python, C++, PHP/Hack, PyTorch, TensorFlow, Spark, Presto, distributed systems, ranking systems, content retrieval, real-time ML</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>TikTok</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ML Engineer Graduate - Multimodal Recommendation (2026 Start)</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>San Jose, CA</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>ML Engineer (Recommendation Systems)</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>https://jobright.ai/jobs/info/68cc15b916d00d2beeb19757</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>BS/MS in Computer Science, ML, or related field; graduating 2026; research experience in multimodal learning or recommendation systems preferred</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Lead multimodal algorithm development for short-video business; explore applications of multimodal technologies in recommendation systems; conduct cutting-edge research in multimodal and MLLM technologies</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Python, PyTorch/TensorFlow, multimodal learning, LLMs, MLLMs, recommendation systems, computer vision, NLP, deep learning, research</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Netflix</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer - Personalization</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Los Gatos, CA</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>ML Engineer (Recommendation Systems)</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>https://explore.jobs.netflix.net/careers/job/790312415414</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>MS/PhD in Computer Science, ML, Statistics, or related field; experience with recommendation systems and personalization at scale</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Design, build, and deploy ML models powering personalized recommendations; develop scalable ML pipelines and infrastructure; work on content optimization, search, and streaming quality</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Python, PyTorch/TensorFlow, recommendation systems, personalization, distributed systems, A/B testing, causal inference, data pipelines, Spark</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Bedrock Robotics</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer: Robotics ML Generalist</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Startup</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>San Francisco, CA / New York, NY</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>https://see.stanford.edu/course/cs229</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Hands-on robotics deployment experience; deep learning expertise for perception and behavior systems</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Deploy ML models to robots; build data labeling pipelines; real-time optimization for robotic systems</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>PyTorch, Python, C++/Rust, ONNX/TensorRT, sensor data processing (camera/lidar/IMU)</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Scale AI</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Machine Learning Research Engineer - Robotics</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>San Francisco, CA</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>https://jobright.ai/jobs/machine-learning-engineer---robotics-jobs-in-united-states</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>3+ years ML experience; ability to take research to production; mid/senior level; H1B possible</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Research and develop ML for robotics applications; bridge research to production systems</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>PyTorch/TensorFlow, reinforcement learning, robotics simulation, research methods</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Toyota Research Institute</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Robotics ML Engineer - Platforms for Vision Language Action</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Los Altos, CA</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>https://jobright.ai/jobs/machine-learning-engineer---robotics-jobs-in-united-states</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Mid/senior level; $176K-$264K salary range; experience with foundation models and robotics platforms</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Build and evaluate learning methods for manipulation; work with Vision-Language-Action (VLA) models</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Foundation models, VLA models, robotics platforms, manipulation learning, PyTorch</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Johnson &amp; Johnson MedTech</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Staff Machine Learning Engineer, Robotics</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Santa Clara, CA</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>https://jobright.ai/jobs/machine-learning-engineer---robotics-jobs-in-united-states</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>6+ years experience; senior/staff level; $141K-$228K; hybrid work; H1B sponsorship</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Deploy ML models for medical robotics; computer vision for surgical applications; edge computing optimization</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>ML deployment, computer vision, edge computing, medical robotics, real-time systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Berkshire Grey</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Principal Robotics Engineer, Machine Learning</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Bedford, MA</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>https://jobright.ai/jobs/machine-learning-engineer---robotics-jobs-in-united-states</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>6+ years robotics/ML experience; senior/lead/staff level; $162K-$200K; near Boston</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Build ML systems for warehouse robotics; scale production autonomy systems</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>ML for robotics, autonomy systems, production scaling, warehouse automation</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Pickle Robot Company</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Perception and Computer Vision Engineer</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Startup</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Boston, MA</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/robotics-engineer-jobs-boston-ma</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Local to Boston area; experience with robotics sensor integration</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Develop computer vision and ML for perception; real-time processing for robotic systems</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Computer vision, ML for perception, robotics sensors, real-time processing, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Diligent Robotics</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Sr ML Engineer, Robotics (Perception)</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Startup</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Austin, TX</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/deep-learning-robotics-jobs</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>5+ years ML/CV experience; senior level; edge deployment expertise</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Build perception systems for healthcare robots; detection and segmentation models; edge deployment</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>PyTorch/TensorFlow, detection/segmentation, edge deployment, healthcare robotics</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>XPENG</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer - LLM, AI &amp; Robotics</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Santa Clara, CA</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>https://jobright.ai/jobs/machine-learning-engineer---robotics-jobs-in-united-states</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Senior level; $149K-$252K; automotive robotics focus</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Develop LLM and AI systems for automotive robotics applications</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>LLMs, robotics AI, deep learning, automotive systems, autonomous vehicles</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Path Robotics</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer, Robot Learning</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Startup</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Columbus, OH</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>https://jobright.ai/jobs/machine-learning-engineer---robotics-jobs-in-united-states</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Mid-level; H1B sponsorship available; industrial automation focus</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Build ML systems for industrial robot automation; imitation and reinforcement learning</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Robot learning, imitation learning, reinforcement learning, industrial automation</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>RobCo</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer - Robot Learning</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Startup</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Europe/US (Remote possible)</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>ML Engineer (Robot Learning)</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>https://robco.jobs.personio.de/job/2450134?language=en</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>ML/robotics intersection experience; ability to deploy to hardware</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Develop learning-based manipulation methods; deploy to real robot hardware; cross-team collaboration</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Learning-based manipulation, systems engineering, hardware deployment, sim-to-real transfer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 10 AI Engineer job listings and synthesized skills section
Add real 2025-2026 AI Engineer postings (Palantir, Quora/Poe, Databricks, Scale AI, Anthropic, Snowflake, Amazon, Google, ServiceNow) to job_listings.xlsx. Create AI Engineer section in skills_aggregate2.md with skill frequency table from 10 listings. Update summary table row. Also includes CLAUDE.md and settings updates from earlier session.
</commit_message>
<xml_diff>
--- a/career/job_listings.xlsx
+++ b/career/job_listings.xlsx
@@ -495,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4338,6 +4338,476 @@
       <c r="I86" t="inlineStr">
         <is>
           <t>Learning-based manipulation, systems engineering, hardware deployment, sim-to-real transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Palantir</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Forward Deployed AI Engineer</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>New York, NY / Washington, DC</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/palantir/636fc05c-d348-4a06-be51-597cb9e07488</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Strong engineering background in CS, Math, Software Engineering, Physics, or ML. Deep understanding of the Gen AI landscape.</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Build end-to-end LLM workflows at scale for enterprise customers. Own Gen AI strategy and implementation. Work directly with customers to solve real-world problems — role resembles a hands-on AI startup CTO. Comfort working in dynamic environments with evolving objectives.</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>Python; LLMs, prompt engineering, agent development; ML fundamentals (evaluation, training, problem decomposition); production Gen AI systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Quora (Poe)</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>AI Engineer New Grad 2025-2026</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Unicorn</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Remote</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>https://jobs.ashbyhq.com/quora/6df58d3e-855a-423e-99fd-a56ac8824b34</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>2025 or Summer 2026 graduate with B.S., M.S., or Ph.D. in CS, Engineering, or related technical field.</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Work on prompt engineering, retrieval-augmented generation, and agentic workflow optimization. Improve existing applied AI systems and identify new opportunities to apply emerging AI capabilities. Take end-to-end ownership from prototyping, data pipelines, model optimization/evaluation to reliable deployment at scale.</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Python, TypeScript; LLM prompt engineering; RAG; agentic workflows; model evaluation and optimization; data pipelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Databricks</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>AI Engineer - FDE (Forward Deployed Engineer)</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Unicorn</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Remote / US</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>https://www.databricks.com/company/careers/professional-services-operations/ai-engineer---fde-forward-deployed-engineer-8024010002</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Graduate degree in CS, Engineering, Statistics, Operations Research, or equivalent practical experience. Passion for driving business value through AI.</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Develop cutting-edge GenAI solutions for customers using latest techniques from Mosaic AI Research. Embed with customer teams from technical ICs to executives. Contribute accelerators, frameworks, and best practices that scale across accounts and influence product roadmap. Travel up to 50%.</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Python, SQL, Java/Scala, JavaScript/TypeScript; AWS/Azure/GCP; Apache Spark; Databricks Intelligence Platform; OpenAI/Anthropic/Gemini APIs; production ML deployments; distributed datasets</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Scale AI</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Applied AI Engineer, Enterprise GenAI</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Unicorn</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>San Francisco, CA / New York, NY</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>https://scale.com/careers/4514173005</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Bachelor's in CS, Mathematics, or related quantitative field. Strong Python proficiency. Cloud platform experience (AWS or GCP).</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Own, plan, and optimize AI behind enterprise customers' deepest technical problems. Build advanced AI agents with multimodal and tool-calling capabilities on Scale's Generative Platform. Convert business requirements into technical implementations. Write and debug production code across company and customer environments.</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Python, NumPy, Pandas; AWS, GCP; LLMs, generative AI applications; AI agents with tool-calling; production ML model development</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Scale AI</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Forward Deployed AI Engineer, Enterprise</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Unicorn</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>San Francisco, CA / New York, NY</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>https://scale.com/careers/4597399005</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>4+ years software engineering experience. Production Python expertise with LangChain, LlamaIndex, HuggingFace, OpenAI API. Cloud platform experience (AWS, GCP, Azure).</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Partner with enterprise clients on infrastructure and data pipeline requirements. Develop production-grade agents for customer support, analysis, content generation, automation. Architect multi-agent systems across models and data sources. Implement RAG systems, fine-tuning pipelines, and human-in-the-loop feedback. Build data connectors and ETL pipelines. Serve as primary technical contact for strategic accounts.</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Python; LangChain, LlamaIndex, HuggingFace, OpenAI API; RAG, embeddings, vector databases; Docker, Kubernetes, CI/CD; Terraform/IaC; multi-agent systems; prompt engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Anthropic</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Forward Deployed Engineer, Applied AI</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Unicorn</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>San Francisco, CA</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>https://job-boards.greenhouse.io/anthropic/jobs/4985877008</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>4+ years experience in a technical, customer-facing role (Forward Deployed Engineer, Solutions Engineer) or as a Software Engineer with consulting experience.</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Production experience with LLMs including advanced prompt engineering and agent development. Work with customers to implement AI solutions that solve their real business problems. Bridge gap between Anthropic's AI capabilities and enterprise customer needs.</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Python; TypeScript, Java; LLMs, advanced prompt engineering; agent development; customer-facing technical implementation</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Snowflake</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Applied AI Engineer</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>San Mateo, CA / Remote</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>https://careers.snowflake.com/us/en/ai-ml-engineering</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Bachelor's in CS, Engineering, or related field. 2+ years professional software engineering experience. Experience in a customer-facing role (solutions architect, sales engineer, or professional services).</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Hands-on builder and critical technical partner to strategic customers at the forefront of enterprise AI. Build, evaluate, and tune applications and pipelines involving ML models or data-intensive systems. Tackle complex and ambiguous technical challenges leveraging cutting-edge research and AI.</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Python; Snowpark, pandas, NumPy; ML model evaluation and tuning; data-intensive pipelines; customer-facing technical delivery</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Software Dev Engineer Intern - AI/ML (Summer 2026), AGI</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>FAANG</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Seattle, WA / Sunnyvale, CA</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>https://www.amazon.jobs/en/jobs/3121382/software-dev-engineer-intern-ai-ml-summer-2026-artificial-general-intelligence-agi</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Enrolled in B.S. or above in CS, Computer Engineering, Data Science, Electrical Engineering, or related STEM field. 18 years or older.</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Experience programming with at least one modern language (Java, C++, Python). Experience with AI/ML technologies. Work on Amazon's Artificial General Intelligence (AGI) organization building next-generation AI products and services.</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Python, Java, C++; AI/ML technologies; cloud platforms (AWS); debugging complex systems; software development lifecycle</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>AI Developer Engineer, Cloud AI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>FAANG</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Sunnyvale, CA / New York, NY / Kirkland, WA</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>https://www.google.com/about/careers/applications/jobs/results/102301475132056262-ai-developer-engineer/</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Bachelor's degree or equivalent practical experience. 2 years experience with software development in Java, Python, or C++, or 1 year with an advanced degree.</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>1 year experience with ML infrastructure (model deployment, evaluation, optimization, data processing, debugging). Experience with GenAI techniques (LLMs, multi-modal, large vision models) or GenAI-related concepts (language modeling, computer vision). Build and deploy AI solutions on Google Cloud for enterprise customers.</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>Python, Java, C++; TensorFlow, PyTorch; ML infrastructure; LLMs, multi-modal models; Google Cloud Platform; model deployment and evaluation</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>ServiceNow</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer Intern - Summer 2026</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Big Tech</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Santa Clara, CA (Hybrid)</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>AI Engineer</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://careers.servicenow.com/jobs/744000080670612/machine-learning-engineer-intern-summer-2026/</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Current enrollment in full-time Bachelor's or Master's in AI, ML, Data Science, CS, or related discipline. Strong theoretical and practical knowledge of ML/deep learning.</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Work alongside engineers to enhance ServiceNow's NLP capabilities using advanced deep learning algorithms. Apply ML to automate enterprise workflows at scale. 12-week internship (May-August or June-September).</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Java, Python, JavaScript, SQL; NumPy, Pandas, Scikit-learn, TensorFlow/PyTorch; supervised/unsupervised learning; model evaluation and optimization; NLP/deep learning</t>
         </is>
       </c>
     </row>

</xml_diff>